<commit_message>
update mapping table & export database
</commit_message>
<xml_diff>
--- a/mapping table rekomendasi.xlsx
+++ b/mapping table rekomendasi.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\XAMPP 7\htdocs\Paket-Wisata-SAW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFCE1A6B-5E4A-4D23-B2EA-9C26D45383EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="-120" windowWidth="19785" windowHeight="11760" xr2:uid="{1540CF5B-7FDB-4078-BAA1-182020ED218B}"/>
+    <workbookView xWindow="1770" yWindow="-120" windowWidth="19785" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>tb_paketwisata</t>
   </si>
@@ -55,9 +54,6 @@
   </si>
   <si>
     <t>kriteria</t>
-  </si>
-  <si>
-    <t>bobot</t>
   </si>
   <si>
     <t>tb_rekomendasi_variabel</t>
@@ -75,7 +71,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -107,7 +103,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -130,14 +126,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,11 +635,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6DE250B-3615-4EBA-8941-1C73EE72435F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,7 +659,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>7</v>
@@ -661,7 +681,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>1</v>
@@ -669,7 +689,7 @@
       <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -681,18 +701,16 @@
         <v>6</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>10</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dokumentasi simple dan mapping table
</commit_message>
<xml_diff>
--- a/mapping table rekomendasi.xlsx
+++ b/mapping table rekomendasi.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1770" yWindow="-120" windowWidth="19785" windowHeight="11760"/>
+    <workbookView xWindow="2715" yWindow="-120" windowWidth="19785" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>tb_paketwisata</t>
   </si>
@@ -66,6 +66,15 @@
   </si>
   <si>
     <t>nama_paketwisata</t>
+  </si>
+  <si>
+    <t>CATATAN</t>
+  </si>
+  <si>
+    <t>tabel yang sudah ada</t>
+  </si>
+  <si>
+    <t>tabel yang ditambahkan</t>
   </si>
 </sst>
 </file>
@@ -89,7 +98,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,8 +111,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -126,38 +147,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -285,16 +286,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1514475</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1514476</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -308,9 +309,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="5610225" y="885825"/>
-          <a:ext cx="723900" cy="209550"/>
+        <a:xfrm flipH="1">
+          <a:off x="3333751" y="1066800"/>
+          <a:ext cx="809624" cy="1352550"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -636,15 +637,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:G8"/>
+  <dimension ref="A4:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
     <col min="5" max="5" width="24.28515625" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" customWidth="1"/>
@@ -652,7 +653,7 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -660,9 +661,6 @@
       </c>
       <c r="E4" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -675,9 +673,6 @@
       <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -689,9 +684,7 @@
       <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -703,7 +696,7 @@
       <c r="E7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="4"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -713,9 +706,41 @@
         <v>12</v>
       </c>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C12" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="6"/>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>